<commit_message>
document rename of verify_email
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -343,12 +343,6 @@
     <t>review_incident_management.php</t>
   </si>
   <si>
-    <t>VerifyEmailAddress.php</t>
-  </si>
-  <si>
-    <t>email_verification.php</t>
-  </si>
-  <si>
     <t>manage\announcement.php</t>
   </si>
   <si>
@@ -392,6 +386,12 @@
   </si>
   <si>
     <t>User-Visible Page</t>
+  </si>
+  <si>
+    <t>verify_email.php</t>
+  </si>
+  <si>
+    <t>verify_emailaddress.php</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -796,10 +796,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -811,7 +811,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
@@ -832,7 +832,7 @@
         <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -852,19 +852,19 @@
         <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
         <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" t="s">
-        <v>116</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
@@ -873,7 +873,7 @@
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -882,10 +882,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -894,7 +894,7 @@
         <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -936,7 +936,7 @@
         <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -957,7 +957,7 @@
         <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -975,7 +975,7 @@
         <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -993,7 +993,7 @@
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1016,7 +1016,7 @@
         <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1037,7 +1037,7 @@
         <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1058,7 +1058,7 @@
         <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1079,7 +1079,7 @@
         <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1100,7 +1100,7 @@
         <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1118,13 +1118,13 @@
         <v>103</v>
       </c>
       <c r="G16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
@@ -1136,16 +1136,16 @@
         <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
@@ -1157,7 +1157,7 @@
         <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1180,7 +1180,7 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1201,7 +1201,7 @@
         <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1222,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1240,7 +1240,7 @@
         <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1258,12 +1258,12 @@
         <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="B24" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
         <v>44</v>
@@ -1272,10 +1272,10 @@
         <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="G24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1296,7 +1296,7 @@
         <v>104</v>
       </c>
       <c r="G25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1316,10 +1316,10 @@
         <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1339,13 +1339,13 @@
         <v>92</v>
       </c>
       <c r="G27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -1357,7 +1357,7 @@
         <v>92</v>
       </c>
       <c r="G28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1368,7 +1368,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
         <v>69</v>
@@ -1380,7 +1380,7 @@
         <v>93</v>
       </c>
       <c r="G29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1398,7 +1398,7 @@
         <v>91</v>
       </c>
       <c r="G30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1415,7 +1415,7 @@
         <v>108</v>
       </c>
       <c r="G31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1432,7 +1432,7 @@
         <v>91</v>
       </c>
       <c r="G32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="2:7">
@@ -1449,7 +1449,7 @@
         <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -1466,7 +1466,7 @@
         <v>92</v>
       </c>
       <c r="G34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:7">
@@ -1483,7 +1483,7 @@
         <v>99</v>
       </c>
       <c r="G35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="2:7">
@@ -1500,7 +1500,7 @@
         <v>94</v>
       </c>
       <c r="G36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="2:7">
@@ -1517,7 +1517,7 @@
         <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="2:7">
@@ -1534,7 +1534,7 @@
         <v>107</v>
       </c>
       <c r="G38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="2:7">
@@ -1551,7 +1551,7 @@
         <v>106</v>
       </c>
       <c r="G39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
document utils and includes
mostly implied already, included for completeness
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="138">
   <si>
     <t>index.php</t>
   </si>
@@ -392,6 +392,42 @@
   </si>
   <si>
     <t>verify_emailaddress.php</t>
+  </si>
+  <si>
+    <t>Utils</t>
+  </si>
+  <si>
+    <t>include_utils\files.php</t>
+  </si>
+  <si>
+    <t>include_utils\procedures.php</t>
+  </si>
+  <si>
+    <t>include_utils\login_functions.php</t>
+  </si>
+  <si>
+    <t>include_utils\date_conversion.php</t>
+  </si>
+  <si>
+    <t>include_utils\email_functions.php</t>
+  </si>
+  <si>
+    <t>include_utils\*.php</t>
+  </si>
+  <si>
+    <t>Wildcard for yet-to-be-determined utility scripts</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>AS NEEDED</t>
+  </si>
+  <si>
+    <t>includes\header.php</t>
+  </si>
+  <si>
+    <t>includes\footer.php</t>
   </si>
 </sst>
 </file>
@@ -775,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -900,19 +936,16 @@
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="G6" t="s">
         <v>119</v>
@@ -921,19 +954,16 @@
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="G7" t="s">
         <v>119</v>
@@ -942,19 +972,19 @@
     <row r="8" spans="1:7">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>119</v>
@@ -963,16 +993,19 @@
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
         <v>119</v>
@@ -981,39 +1014,37 @@
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
       </c>
       <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
         <v>119</v>
@@ -1022,31 +1053,30 @@
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
@@ -1064,10 +1094,10 @@
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -1085,10 +1115,10 @@
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
@@ -1106,7 +1136,10 @@
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1115,7 +1148,7 @@
         <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
         <v>119</v>
@@ -1124,7 +1157,10 @@
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
@@ -1142,10 +1178,7 @@
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
@@ -1154,30 +1187,25 @@
         <v>53</v>
       </c>
       <c r="F18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2"/>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
         <v>90</v>
-      </c>
-      <c r="G18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2</v>
       </c>
       <c r="G19" t="s">
         <v>119</v>
@@ -1186,40 +1214,42 @@
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G21" t="s">
         <v>119</v>
@@ -1228,16 +1258,19 @@
     <row r="22" spans="1:7">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
         <v>119</v>
@@ -1246,33 +1279,37 @@
     <row r="23" spans="1:7">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
       </c>
       <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2"/>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="B24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="G24" t="s">
         <v>119</v>
@@ -1281,80 +1318,77 @@
     <row r="25" spans="1:7">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2"/>
+      <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>20</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>44</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>57</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F27" t="s">
         <v>104</v>
       </c>
-      <c r="G25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
+      <c r="G27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>43</v>
-      </c>
-      <c r="D26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" t="s">
-        <v>122</v>
-      </c>
-      <c r="G26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2"/>
-      <c r="B28" t="s">
-        <v>109</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
         <v>119</v>
@@ -1362,22 +1396,19 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G29" t="s">
         <v>119</v>
@@ -1386,47 +1417,54 @@
     <row r="30" spans="1:7">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G30" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>117</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="G31" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7">
+      <c r="A32" s="2"/>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F32" t="s">
         <v>91</v>
@@ -1435,123 +1473,262 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="G33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G34" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G35" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="E36" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
         <v>81</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F38" t="s">
         <v>94</v>
       </c>
-      <c r="G36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" t="s">
+      <c r="G38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="B39" t="s">
         <v>83</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D39" t="s">
         <v>84</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E39" t="s">
         <v>95</v>
-      </c>
-      <c r="F37" t="s">
-        <v>106</v>
-      </c>
-      <c r="G37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7">
-      <c r="B38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" t="s">
-        <v>96</v>
-      </c>
-      <c r="F38" t="s">
-        <v>107</v>
-      </c>
-      <c r="G38" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" t="s">
-        <v>97</v>
       </c>
       <c r="F39" t="s">
         <v>106</v>
       </c>
       <c r="G39" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>128</v>
+      </c>
+      <c r="G42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>127</v>
+      </c>
+      <c r="G43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="B44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="B45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>130</v>
+      </c>
+      <c r="G45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="B46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
document Editor user-management list and related new pages
addition of deactivate_user.php, editor_find_users.php,
editor_user_account_management.php
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="143">
   <si>
     <t>index.php</t>
   </si>
@@ -331,9 +331,6 @@
     <t>account_management.php, account_settings.php, user_update_email.php</t>
   </si>
   <si>
-    <t>account_management.php, editor_create_user.php</t>
-  </si>
-  <si>
     <t>editor_view_submissions.php</t>
   </si>
   <si>
@@ -428,6 +425,24 @@
   </si>
   <si>
     <t>includes\footer.php</t>
+  </si>
+  <si>
+    <t>account_management.php, editor_create_user.php, deactivate_user.php, editor_user_account_management.php</t>
+  </si>
+  <si>
+    <t>editor_find_users.php</t>
+  </si>
+  <si>
+    <t>manage\user_accounts.php</t>
+  </si>
+  <si>
+    <t>Editor list of users</t>
+  </si>
+  <si>
+    <t>editor_user_account_management.php, editor_find_users.php</t>
+  </si>
+  <si>
+    <t>Editor making adding or changing a single user *merge pages for processing updates*</t>
   </si>
 </sst>
 </file>
@@ -811,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -832,10 +847,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -847,7 +862,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
@@ -868,7 +883,7 @@
         <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -888,19 +903,19 @@
         <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
         <v>112</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>113</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
@@ -909,7 +924,7 @@
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -918,10 +933,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -930,13 +945,13 @@
         <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
@@ -945,16 +960,16 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -963,10 +978,10 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -987,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1008,7 +1023,7 @@
         <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1029,7 +1044,7 @@
         <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1047,7 +1062,7 @@
         <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1065,7 +1080,7 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1088,7 +1103,7 @@
         <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1109,7 +1124,7 @@
         <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1130,7 +1145,7 @@
         <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1151,7 +1166,7 @@
         <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1172,7 +1187,7 @@
         <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1190,13 +1205,13 @@
         <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
@@ -1208,16 +1223,16 @@
         <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
@@ -1229,7 +1244,7 @@
         <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1252,7 +1267,7 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1273,7 +1288,7 @@
         <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1294,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1309,10 +1324,10 @@
         <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1320,6 +1335,9 @@
       <c r="B25" t="s">
         <v>64</v>
       </c>
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
@@ -1327,97 +1345,97 @@
         <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7">
+      <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>139</v>
+      </c>
+      <c r="C26" t="s">
+        <v>140</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="G26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="2"/>
       <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="D27" t="s">
         <v>44</v>
       </c>
       <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2"/>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
         <v>57</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>104</v>
       </c>
-      <c r="G27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" t="s">
-        <v>122</v>
-      </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -1429,224 +1447,225 @@
         <v>92</v>
       </c>
       <c r="G30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="C31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
         <v>69</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>93</v>
       </c>
-      <c r="G31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="2"/>
-      <c r="B32" t="s">
+      <c r="G32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2"/>
+      <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>75</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>91</v>
       </c>
-      <c r="G32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" t="s">
-        <v>108</v>
-      </c>
       <c r="G33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F36" t="s">
         <v>92</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="F37" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F39" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F41" t="s">
         <v>106</v>
       </c>
       <c r="G41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="F42" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="G42" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7">
+      <c r="A43" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="B43" t="s">
         <v>127</v>
       </c>
@@ -1660,12 +1679,12 @@
         <v>127</v>
       </c>
       <c r="G43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D44" t="s">
         <v>36</v>
@@ -1674,15 +1693,15 @@
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
         <v>36</v>
@@ -1691,15 +1710,15 @@
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -1708,18 +1727,15 @@
         <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
         <v>36</v>
@@ -1727,8 +1743,28 @@
       <c r="E47" t="s">
         <v>45</v>
       </c>
+      <c r="F47" t="s">
+        <v>130</v>
+      </c>
       <c r="G47" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+      <c r="G48" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial check-in of review_submission.php
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="144">
   <si>
     <t>index.php</t>
   </si>
@@ -337,9 +337,6 @@
     <t>author_incident_management.php, view_feedback.php, author_view_feedback.php, editor_view_submissions.php</t>
   </si>
   <si>
-    <t>review_incident_management.php</t>
-  </si>
-  <si>
     <t>manage\announcement.php</t>
   </si>
   <si>
@@ -443,6 +440,12 @@
   </si>
   <si>
     <t>Editor making adding or changing a single user *merge pages for processing updates*</t>
+  </si>
+  <si>
+    <t>NEW, review_incident_management.php</t>
+  </si>
+  <si>
+    <t>IN PROGRESS - NEW FILE - Mitch Spencer</t>
   </si>
 </sst>
 </file>
@@ -828,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -847,10 +850,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -862,7 +865,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
@@ -883,7 +886,7 @@
         <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -903,19 +906,19 @@
         <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
         <v>111</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>112</v>
-      </c>
-      <c r="D4" t="s">
-        <v>113</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
@@ -924,7 +927,7 @@
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -933,10 +936,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -945,13 +948,13 @@
         <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
@@ -960,16 +963,16 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -978,10 +981,10 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1002,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1023,7 +1026,7 @@
         <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1044,7 +1047,7 @@
         <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1062,7 +1065,7 @@
         <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1080,7 +1083,7 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1103,7 +1106,7 @@
         <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1124,7 +1127,7 @@
         <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1145,7 +1148,7 @@
         <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1166,7 +1169,7 @@
         <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1187,7 +1190,7 @@
         <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1205,13 +1208,13 @@
         <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
@@ -1223,16 +1226,16 @@
         <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
@@ -1244,7 +1247,7 @@
         <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1267,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1288,7 +1291,7 @@
         <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1309,7 +1312,7 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1324,10 +1327,10 @@
         <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1336,7 +1339,7 @@
         <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1345,33 +1348,33 @@
         <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" t="s">
         <v>139</v>
-      </c>
-      <c r="C26" t="s">
-        <v>140</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" t="s">
         <v>44</v>
@@ -1380,10 +1383,10 @@
         <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1404,7 +1407,7 @@
         <v>104</v>
       </c>
       <c r="G28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1424,10 +1427,10 @@
         <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1447,13 +1450,13 @@
         <v>92</v>
       </c>
       <c r="G30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
@@ -1465,7 +1468,7 @@
         <v>92</v>
       </c>
       <c r="G31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1476,7 +1479,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
         <v>69</v>
@@ -1488,7 +1491,7 @@
         <v>93</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1506,7 +1509,7 @@
         <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1520,10 +1523,10 @@
         <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1540,7 +1543,7 @@
         <v>91</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1557,7 +1560,7 @@
         <v>92</v>
       </c>
       <c r="G36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1574,7 +1577,7 @@
         <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1591,7 +1594,7 @@
         <v>99</v>
       </c>
       <c r="G38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1608,7 +1611,7 @@
         <v>94</v>
       </c>
       <c r="G39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1625,7 +1628,7 @@
         <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1642,7 +1645,7 @@
         <v>106</v>
       </c>
       <c r="G41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1659,15 +1662,15 @@
         <v>105</v>
       </c>
       <c r="G42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
         <v>36</v>
@@ -1676,15 +1679,15 @@
         <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D44" t="s">
         <v>36</v>
@@ -1693,15 +1696,15 @@
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D45" t="s">
         <v>36</v>
@@ -1710,15 +1713,15 @@
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -1727,15 +1730,15 @@
         <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
         <v>36</v>
@@ -1744,18 +1747,18 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
         <v>131</v>
-      </c>
-      <c r="C48" t="s">
-        <v>132</v>
       </c>
       <c r="D48" t="s">
         <v>36</v>
@@ -1764,7 +1767,7 @@
         <v>45</v>
       </c>
       <c r="G48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change page names so subfolders are not needed
time constraints mean technical issue of includes from different
folder-levels won't be addressed
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -79,18 +79,9 @@
     <t>Changes settings for the User</t>
   </si>
   <si>
-    <t>search\users.php</t>
-  </si>
-  <si>
     <t>search\critical_incidents.php</t>
   </si>
   <si>
-    <t>settings\account.php</t>
-  </si>
-  <si>
-    <t>settings\system.php</t>
-  </si>
-  <si>
     <t>includes\dashboard.php</t>
   </si>
   <si>
@@ -109,21 +100,6 @@
     <t>Info</t>
   </si>
   <si>
-    <t>about\submission.php</t>
-  </si>
-  <si>
-    <t>about\reviews.php</t>
-  </si>
-  <si>
-    <t>about\cabells.php</t>
-  </si>
-  <si>
-    <t>about\conference.php</t>
-  </si>
-  <si>
-    <t>about\contact.php</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
@@ -193,9 +169,6 @@
     <t>E10, E11, E12, E13</t>
   </si>
   <si>
-    <t>view\critical_incident.php</t>
-  </si>
-  <si>
     <t>G40, G41, G43</t>
   </si>
   <si>
@@ -208,18 +181,12 @@
     <t>Submissions</t>
   </si>
   <si>
-    <t>manage\update_user.php</t>
-  </si>
-  <si>
     <t>E23, E24, E25, E26, E27, E28</t>
   </si>
   <si>
     <t>Announcements</t>
   </si>
   <si>
-    <t>settings\announcements.php</t>
-  </si>
-  <si>
     <t>E30, E31, E32, E33, E34, E35, E36, E37</t>
   </si>
   <si>
@@ -232,9 +199,6 @@
     <t>Reviewer</t>
   </si>
   <si>
-    <t>manage\author_submission.php</t>
-  </si>
-  <si>
     <t>C40, A10, C43</t>
   </si>
   <si>
@@ -244,42 +208,24 @@
     <t>C40, E41, E43, E44, E46, C43, C50, G42</t>
   </si>
   <si>
-    <t>manage\reviewer_submission.php</t>
-  </si>
-  <si>
     <t>C40, E41, G42, C43, C50</t>
   </si>
   <si>
     <t>publish_submission.php</t>
   </si>
   <si>
-    <t>manage\journal.php</t>
-  </si>
-  <si>
     <t>E43, G42, C43, C50</t>
   </si>
   <si>
     <t>E45</t>
   </si>
   <si>
-    <t>manage\assign_reviewers.php</t>
-  </si>
-  <si>
-    <t>view\author_submissions.php</t>
-  </si>
-  <si>
     <t>Reviewer, Editor</t>
   </si>
   <si>
-    <t>view\reviewer_submissions.php</t>
-  </si>
-  <si>
     <t>E43</t>
   </si>
   <si>
-    <t>view\ready_to_publish.php</t>
-  </si>
-  <si>
     <t>includes\sidebar.php, includes\subnav.php, author_incident_management.php (author tab), editor_incident_management.php (editor tab), reviewer_incident_management.php (reviewer tab)</t>
   </si>
   <si>
@@ -310,9 +256,6 @@
     <t>C40, E41, E43, E46, C50</t>
   </si>
   <si>
-    <t>manage\assign_editor.php</t>
-  </si>
-  <si>
     <t>assign_editor.php</t>
   </si>
   <si>
@@ -322,9 +265,6 @@
     <t>index.php, logged_in.php, editor_index.php</t>
   </si>
   <si>
-    <t>about\teaching_notes.php</t>
-  </si>
-  <si>
     <t>teaching_notes.php</t>
   </si>
   <si>
@@ -337,15 +277,6 @@
     <t>author_incident_management.php, view_feedback.php, author_view_feedback.php, editor_view_submissions.php</t>
   </si>
   <si>
-    <t>manage\announcement.php</t>
-  </si>
-  <si>
-    <t>about\authors.php</t>
-  </si>
-  <si>
-    <t>about\*.php</t>
-  </si>
-  <si>
     <t>includes\sidebar.php</t>
   </si>
   <si>
@@ -427,9 +358,6 @@
     <t>editor_find_users.php</t>
   </si>
   <si>
-    <t>manage\user_accounts.php</t>
-  </si>
-  <si>
     <t>Editor list of users</t>
   </si>
   <si>
@@ -449,6 +377,78 @@
   </si>
   <si>
     <t>account_management.php, editor_create_user.php, deactivate_user.php, editor_user_account_management.php, editor_update_user.php</t>
+  </si>
+  <si>
+    <t>view_critical_incident.php</t>
+  </si>
+  <si>
+    <t>about_submission.php</t>
+  </si>
+  <si>
+    <t>about_reviews.php</t>
+  </si>
+  <si>
+    <t>about_cabells.php</t>
+  </si>
+  <si>
+    <t>about_conference.php</t>
+  </si>
+  <si>
+    <t>about_contact.php</t>
+  </si>
+  <si>
+    <t>about_teaching_notes.php</t>
+  </si>
+  <si>
+    <t>about_authors.php</t>
+  </si>
+  <si>
+    <t>about_*.php</t>
+  </si>
+  <si>
+    <t>search_users.php</t>
+  </si>
+  <si>
+    <t>manage_update_user.php</t>
+  </si>
+  <si>
+    <t>manage_user_accounts.php</t>
+  </si>
+  <si>
+    <t>settings_account.php</t>
+  </si>
+  <si>
+    <t>settings_system.php</t>
+  </si>
+  <si>
+    <t>settings_announcements.php</t>
+  </si>
+  <si>
+    <t>manage_announcement.php</t>
+  </si>
+  <si>
+    <t>manage_author_submission.php</t>
+  </si>
+  <si>
+    <t>manage_reviewer_submission.php</t>
+  </si>
+  <si>
+    <t>manage_journal.php</t>
+  </si>
+  <si>
+    <t>manage_assign_editor.php</t>
+  </si>
+  <si>
+    <t>manage_assign_reviewers.php</t>
+  </si>
+  <si>
+    <t>view_author_submissions.php</t>
+  </si>
+  <si>
+    <t>view_reviewer_submissions.php</t>
+  </si>
+  <si>
+    <t>view_ready_to_publish.php</t>
   </si>
 </sst>
 </file>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -853,22 +853,22 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
@@ -883,13 +883,13 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -900,94 +900,94 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -999,16 +999,16 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1017,19 +1017,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1038,219 +1038,219 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1264,16 +1264,16 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1285,16 +1285,16 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1306,111 +1306,111 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="G24" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="G25" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="G26" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1418,359 +1418,359 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="G29" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G32" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2"/>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="G34" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F35" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G36" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F37" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G37" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="G38" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="G39" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="F40" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G40" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="F41" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G41" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>87</v>
+        <v>144</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F42" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G42" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="G43" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F44" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F45" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="G45" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E46" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F46" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="G46" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E47" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F47" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G48" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missed search_critical_incidents folder update
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -79,9 +79,6 @@
     <t>Changes settings for the User</t>
   </si>
   <si>
-    <t>search\critical_incidents.php</t>
-  </si>
-  <si>
     <t>includes\dashboard.php</t>
   </si>
   <si>
@@ -449,6 +446,9 @@
   </si>
   <si>
     <t>view_ready_to_publish.php</t>
+  </si>
+  <si>
+    <t>search_critical_incidents.php</t>
   </si>
 </sst>
 </file>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -853,22 +853,22 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
@@ -883,13 +883,13 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -900,94 +900,94 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
         <v>87</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s">
-        <v>89</v>
-      </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
         <v>89</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -999,16 +999,16 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1017,19 +1017,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1038,219 +1038,219 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1264,16 +1264,16 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1285,16 +1285,16 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1306,111 +1306,111 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
         <v>99</v>
       </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" t="s">
-        <v>100</v>
-      </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1418,359 +1418,359 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2"/>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" t="s">
         <v>59</v>
       </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G34" t="s">
         <v>117</v>
-      </c>
-      <c r="G34" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
         <v>107</v>
       </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
       <c r="D48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to pagemap statuses
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="148">
   <si>
     <t>index.php</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Which pages are likely to be refactored into this page</t>
   </si>
   <si>
-    <t>login.php; login_page.php</t>
-  </si>
-  <si>
     <t>Info</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>includes\sidebar.php, includes\subnav.php, author_incident_management.php (author tab), editor_incident_management.php (editor tab), reviewer_incident_management.php (reviewer tab)</t>
   </si>
   <si>
-    <t>search_cases.php</t>
-  </si>
-  <si>
     <t>NEW</t>
   </si>
   <si>
@@ -367,9 +361,6 @@
     <t>NEW, review_incident_management.php</t>
   </si>
   <si>
-    <t>IN PROGRESS - NEW FILE - Mitch Spencer</t>
-  </si>
-  <si>
     <t>contact.php</t>
   </si>
   <si>
@@ -449,6 +440,24 @@
   </si>
   <si>
     <t>search_critical_incidents.php</t>
+  </si>
+  <si>
+    <t>REEVALUATE</t>
+  </si>
+  <si>
+    <t>login.php; login_page.php, logged_in.php</t>
+  </si>
+  <si>
+    <t>VALIDATE</t>
+  </si>
+  <si>
+    <t>create_announcement.php</t>
+  </si>
+  <si>
+    <t>manage_announcements.php</t>
+  </si>
+  <si>
+    <t>IN PROGRESS - NEW PAGE - Mitch Spencer</t>
   </si>
 </sst>
 </file>
@@ -832,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -853,10 +862,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -868,7 +877,7 @@
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1">
@@ -883,13 +892,13 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -900,37 +909,37 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
         <v>86</v>
       </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>88</v>
-      </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -939,55 +948,55 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -999,16 +1008,16 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1017,19 +1026,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1038,219 +1047,216 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
         <v>144</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1264,16 +1270,16 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1285,16 +1291,16 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="G22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1306,111 +1312,111 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1418,359 +1424,374 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
       <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2"/>
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" t="s">
+        <v>146</v>
+      </c>
+      <c r="G32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
         <v>56</v>
       </c>
-      <c r="F31" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="2"/>
-      <c r="B33" t="s">
-        <v>136</v>
-      </c>
-      <c r="D33" t="s">
-        <v>14</v>
-      </c>
       <c r="E33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
         <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:7">
+      <c r="A34" s="2"/>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
         <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F35" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="G35" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F38" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F40" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="G40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E41" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" t="s">
         <v>14</v>
       </c>
-      <c r="E42" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="2" t="s">
+      <c r="E43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
         <v>100</v>
       </c>
-      <c r="B43" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" t="s">
-        <v>36</v>
-      </c>
-      <c r="F43" t="s">
-        <v>102</v>
-      </c>
-      <c r="G43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="B44" t="s">
-        <v>101</v>
-      </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F47" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" t="s">
+        <v>103</v>
+      </c>
+      <c r="G48" t="s">
         <v>106</v>
       </c>
-      <c r="C48" t="s">
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49" t="s">
         <v>107</v>
-      </c>
-      <c r="D48" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" t="s">
-        <v>36</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
status updates for mapping document
</commit_message>
<xml_diff>
--- a/project_documents/refactor_pagemap.xlsx
+++ b/project_documents/refactor_pagemap.xlsx
@@ -457,9 +457,6 @@
     <t>manage_announcements.php</t>
   </si>
   <si>
-    <t>IN PROGRESS - NEW PAGE - Mitch Spencer</t>
-  </si>
-  <si>
     <t>Editor cleans up author files for double-blind</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>List Author submissions, links to different management pages based on status</t>
+  </si>
+  <si>
+    <t>FINISH CODE</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1124,7 +1124,7 @@
         <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1145,7 +1145,7 @@
         <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1166,7 +1166,7 @@
         <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1187,7 +1187,7 @@
         <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1208,7 +1208,7 @@
         <v>115</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1226,7 +1226,7 @@
         <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1244,7 +1244,7 @@
         <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1265,7 +1265,7 @@
         <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1288,7 +1288,7 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1330,7 +1330,7 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1425,7 +1425,7 @@
         <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1448,7 +1448,7 @@
         <v>94</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1533,7 +1533,7 @@
         <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
@@ -1545,7 +1545,7 @@
         <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1579,7 +1579,7 @@
         <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1596,7 +1596,7 @@
         <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1613,7 +1613,7 @@
         <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1655,7 +1655,7 @@
         <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D41" t="s">
         <v>66</v>
@@ -1684,7 +1684,7 @@
         <v>83</v>
       </c>
       <c r="G42" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:7">

</xml_diff>